<commit_message>
Fix index.md. Update cat_ref.xlsx and HIS data
</commit_message>
<xml_diff>
--- a/cat_ref.xlsx
+++ b/cat_ref.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="559">
   <si>
     <t>code</t>
   </si>
@@ -1769,6 +1769,13 @@
   </si>
   <si>
     <t>Other Hematological Agents</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>on-09-07</t>
+  </si>
+  <si>
+    <t>Trop-2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2156,10 +2163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B279"/>
+  <dimension ref="A1:B280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4035,369 +4042,377 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>343</v>
+        <v>557</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>329</v>
+        <v>558</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>522</v>
+        <v>343</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>523</v>
+        <v>329</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>344</v>
+        <v>528</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>346</v>
+        <v>530</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>531</v>
+        <v>348</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>351</v>
+        <v>531</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>532</v>
+        <v>355</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>430</v>
+        <v>532</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>533</v>
+        <v>430</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>537</v>
+        <v>361</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>362</v>
+        <v>537</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>363</v>
+        <v>538</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>539</v>
+        <v>365</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>368</v>
+        <v>539</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>540</v>
+        <v>378</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>385</v>
+        <v>544</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>545</v>
+        <v>385</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>391</v>
+        <v>548</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>549</v>
+        <v>395</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>550</v>
+        <v>396</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>397</v>
+        <v>550</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>398</v>
+        <v>551</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>552</v>
+        <v>397</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>553</v>
+        <v>398</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B279" s="2" t="s">
+      <c r="B280" s="2" t="s">
         <v>554</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update category reference file.
</commit_message>
<xml_diff>
--- a/cat_ref.xlsx
+++ b/cat_ref.xlsx
@@ -2278,14 +2278,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.28515625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="10.28515625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add new category ON-09-09 and update changelog
</commit_message>
<xml_diff>
--- a/cat_ref.xlsx
+++ b/cat_ref.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="577">
   <si>
     <t>code</t>
   </si>
@@ -1899,6 +1899,13 @@
   <si>
     <t>Specific Antirheumatic Agents</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>on-09-09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anti-CTLA-4</t>
   </si>
 </sst>
 </file>
@@ -2284,10 +2291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B288"/>
+  <dimension ref="A1:B289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A230" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E241" sqref="E241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4234,369 +4241,377 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>292</v>
+        <v>575</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>278</v>
+        <v>576</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>451</v>
+        <v>292</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>452</v>
+        <v>278</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>293</v>
+        <v>457</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>564</v>
+        <v>293</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>565</v>
+        <v>459</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>294</v>
+        <v>564</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>295</v>
+        <v>565</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>460</v>
+        <v>295</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>298</v>
+        <v>460</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>461</v>
+        <v>302</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>366</v>
+        <v>461</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>462</v>
+        <v>366</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>466</v>
+        <v>308</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>309</v>
+        <v>466</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>310</v>
+        <v>467</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>468</v>
+        <v>312</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>566</v>
+        <v>313</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>567</v>
+        <v>468</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>314</v>
+        <v>566</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>315</v>
+        <v>567</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>469</v>
+        <v>323</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>568</v>
+        <v>328</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>569</v>
+        <v>473</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>329</v>
+        <v>568</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>474</v>
+        <v>569</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>334</v>
+        <v>477</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
-        <v>570</v>
+        <v>333</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>571</v>
+        <v>334</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>335</v>
+        <v>571</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>336</v>
+        <v>572</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>513</v>
+        <v>335</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
-        <v>478</v>
+        <v>336</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>479</v>
+        <v>513</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>337</v>
+        <v>478</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>338</v>
+        <v>479</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>480</v>
+        <v>337</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>481</v>
+        <v>338</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B288" s="2" t="s">
+      <c r="B289" s="2" t="s">
         <v>482</v>
       </c>
     </row>

</xml_diff>